<commit_message>
test full procedure of extracting data for one category and uploading it to s3.
</commit_message>
<xml_diff>
--- a/data/Store_Category_Sheet_test.xlsx
+++ b/data/Store_Category_Sheet_test.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Open Delta Youtube\Python\aws_webscrape\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91B7F094-818A-4F0E-93C7-98AC73F69EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Woolworths" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Woolworths"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Categories</t>
   </si>
@@ -34,16 +28,14 @@
     <t>https://www.woolworths.co.za/cat/Food/Fruit-Vegetables-Salads/_/N-lllnam</t>
   </si>
   <si>
-    <t>Meat, Poultry &amp; Fish</t>
-  </si>
-  <si>
-    <t>https://www.woolworths.co.za/cat/Food/Meat-Poultry-Fish/_/N-d87rb7</t>
+    <t/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -61,7 +53,7 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF0000ff"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -93,42 +85,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="6">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:B8" totalsRowShown="0">
-  <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B8" displayName="Table_1" name="Table_1" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:B8"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Categories"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="URLs"/>
+    <tableColumn name="Categories" id="1"/>
+    <tableColumn name="URLs" id="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="1" showFirstColumn="1"/>
 </table>
 </file>
 
@@ -137,10 +132,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -178,71 +173,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -270,7 +265,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -293,11 +288,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -306,13 +301,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -322,7 +317,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -331,7 +326,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -340,7 +335,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -348,10 +343,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -416,65 +411,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="93.57642857142856" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>